<commit_message>
Atualização de Lista de Requisitos
</commit_message>
<xml_diff>
--- a/02 Especificação de Requisitos.xlsx
+++ b/02 Especificação de Requisitos.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\extraeletro\Documents\ANALISE\Trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="61">
   <si>
     <t>Nº</t>
   </si>
@@ -32,12 +32,6 @@
     <t>Ator</t>
   </si>
   <si>
-    <t>Marcar Consulta</t>
-  </si>
-  <si>
-    <t>Desmarcar Consulta</t>
-  </si>
-  <si>
     <t>Pagar Consulta</t>
   </si>
   <si>
@@ -47,9 +41,6 @@
     <t>Logar</t>
   </si>
   <si>
-    <t>Remarcar Consulta</t>
-  </si>
-  <si>
     <t>Manter Paciente</t>
   </si>
   <si>
@@ -92,9 +83,6 @@
     <t>UC 04</t>
   </si>
   <si>
-    <t>Manter Agenda de Atendimento</t>
-  </si>
-  <si>
     <t>UC 05</t>
   </si>
   <si>
@@ -146,12 +134,6 @@
     <t>UC 17</t>
   </si>
   <si>
-    <t>UC 18</t>
-  </si>
-  <si>
-    <t>UC 19</t>
-  </si>
-  <si>
     <t>Atendente | Gerente | Médico</t>
   </si>
   <si>
@@ -164,9 +146,6 @@
     <t>Gerar Atestado Médico</t>
   </si>
   <si>
-    <t>UC 20</t>
-  </si>
-  <si>
     <t>Consultar Atendimentos agendados</t>
   </si>
   <si>
@@ -176,21 +155,6 @@
     <t>Identificar os usuários: Para que os usuários possam acessar as funcionalidades do sistema, com base em suas respectivas permissões é necessário que estejam “logados”;</t>
   </si>
   <si>
-    <t>O sistema deverá permitir aos usuários autorizados marcar consultas;</t>
-  </si>
-  <si>
-    <t>O Sistema deverá permitir aos usuários autorizados desmarcar a consulta agendada;</t>
-  </si>
-  <si>
-    <t>O sistema deverá permitir aos usuários autorizados remarcar a consulta agendada;</t>
-  </si>
-  <si>
-    <t>O sistema deverá permitir, ao marcar ou remarcar a consulta, que os usuários Consultar e/ou editar a agenda do médico;</t>
-  </si>
-  <si>
-    <t>O sistema deverá permitir aos usuários autorizados, ao chegar o paciente para ser atendido, cadastrar ou atualizar os dados do paciente;</t>
-  </si>
-  <si>
     <t>O sistema deverá permiti aos usuários autorizados, gerar pagamento paras as consultas registradas;</t>
   </si>
   <si>
@@ -234,6 +198,15 @@
   </si>
   <si>
     <t>Descrição</t>
+  </si>
+  <si>
+    <t>Agendar, remarcar, desmarcar e consultar agendamentos de consultas.</t>
+  </si>
+  <si>
+    <t>Manter Agenda de Atendimento Médicos.</t>
+  </si>
+  <si>
+    <t>O sistema permitirá ao atendente confirmar a presença do paciente e incluí-lo em uma fila de atendimento.</t>
   </si>
 </sst>
 </file>
@@ -298,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -318,9 +291,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -331,10 +301,10 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -644,31 +614,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E22" sqref="A1:E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="77.140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" style="9" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="36.7109375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="36.7109375" style="8" customWidth="1"/>
     <col min="6" max="6" width="3.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10" t="s">
         <v>1</v>
       </c>
     </row>
@@ -678,42 +648,42 @@
         <v>0</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" s="12"/>
+        <v>57</v>
+      </c>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>2</v>
+        <v>16</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>59</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -721,16 +691,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>3</v>
+        <v>17</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>5</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -738,16 +708,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>7</v>
+        <v>18</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -755,16 +725,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -772,16 +742,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>8</v>
+        <v>20</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>2</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -789,16 +759,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>12</v>
+        <v>21</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -806,16 +776,16 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>13</v>
+        <v>22</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -823,16 +793,16 @@
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -840,16 +810,16 @@
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>14</v>
+        <v>24</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -857,16 +827,16 @@
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>43</v>
+        <v>25</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -874,16 +844,16 @@
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="C14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -891,16 +861,16 @@
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>9</v>
+        <v>29</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -908,13 +878,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>10</v>
+        <v>31</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>34</v>
@@ -925,13 +895,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>11</v>
+        <v>32</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>34</v>
@@ -942,13 +912,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>44</v>
+        <v>33</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>34</v>
@@ -959,67 +929,16 @@
         <v>17</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>16</v>
+        <v>35</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>40</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>18</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>19</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>20</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correção de erros no UC02 e UC05.
Correção de erros no UC02 e UC05.
</commit_message>
<xml_diff>
--- a/02 Especificação de Requisitos.xlsx
+++ b/02 Especificação de Requisitos.xlsx
@@ -617,7 +617,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,7 +683,7 @@
         <v>59</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -734,7 +734,7 @@
         <v>10</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>